<commit_message>
thay đổi giao diện thời khóa biểu
</commit_message>
<xml_diff>
--- a/backend/test_output.xlsx
+++ b/backend/test_output.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tổng quan" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Chi tiết lớp học" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Phương án 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,32 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="004472C4"/>
-      <sz val="16"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="0028A745"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FF6B00"/>
-      <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
@@ -83,13 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -461,198 +437,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>PHƯƠNG ÁN 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>THÔNG TIN SINH VIÊN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Kỳ học:</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>CPA:</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3.45</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>ĐIỂM PHƯƠNG ÁN</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Điểm tổng:</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>145.58/100</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>CHỈ SỐ LỊCH HỌC</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tổng số môn:</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4 môn</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tổng tín chỉ:</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>7 TC</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Số ngày học/tuần:</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2 ngày</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Số ngày nghỉ/tuần:</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5 ngày</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Trung bình giờ/ngày:</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>8.2 giờ</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Giờ học sớm nhất:</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>06:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Giờ học muộn nhất:</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>17:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Ngày học liên tục (&gt;5h):</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2 ngày</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>⭐ PHƯƠNG ÁN ĐƯỢC KHUYÊN DÙNG</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A20:D20"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -673,210 +457,210 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Mã lớp</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Tên lớp</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Thời gian</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Ngày học</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Tuần học</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Phòng</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Giáo viên</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Ghi chú</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>166141</t>
         </is>
       </c>
-      <c r="B2" s="7" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Tiếng Nhật 8</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>08:25 - 10:05</t>
         </is>
       </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="E2" s="7" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>25, 26, 27, 28, 29, 30, 31, 32, 34, 35, 36, 37, 38, 39, 40, 41, 42</t>
         </is>
       </c>
-      <c r="F2" s="6" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>C7-217</t>
         </is>
       </c>
-      <c r="G2" s="7" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>TBA</t>
         </is>
       </c>
-      <c r="H2" s="7" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>Matches semester 8</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>166138</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Kỹ năng ITSS học bằng tiếng Nhật 2</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>14:10 - 17:30</t>
         </is>
       </c>
-      <c r="D3" s="6" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>25, 26, 27, 28, 29, 30, 31, 32, 34, 35, 36, 37, 38, 39, 40, 41, 42</t>
         </is>
       </c>
-      <c r="F3" s="6" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>B1-201</t>
         </is>
       </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>TBA</t>
         </is>
       </c>
-      <c r="H3" s="7" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>Matches semester 8</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>167910</t>
         </is>
       </c>
-      <c r="B4" s="7" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Quản trị phát triển phần mềm</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>12:30 - 14:00</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="E4" s="7" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>25, 26, 27, 28, 29, 30, 31, 32, 34, 35, 36, 37, 38, 39, 40, 41, 42</t>
         </is>
       </c>
-      <c r="F4" s="6" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>D9-402</t>
         </is>
       </c>
-      <c r="G4" s="7" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>TBA</t>
         </is>
       </c>
-      <c r="H4" s="7" t="inlineStr">
+      <c r="H4" s="3" t="inlineStr">
         <is>
           <t>Matches semester 8</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>168499</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Nhập môn Khoa học dữ liệu</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>06:45 - 09:10</t>
         </is>
       </c>
-      <c r="D5" s="6" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>25, 26, 27, 28, 29, 30, 31, 32, 34, 35, 36, 37, 38, 39, 40, 41, 42</t>
         </is>
       </c>
-      <c r="F5" s="6" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>TC-307</t>
         </is>
       </c>
-      <c r="G5" s="7" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>TBA</t>
         </is>
       </c>
-      <c r="H5" s="7" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t>Matches semester 8</t>
         </is>

</xml_diff>